<commit_message>
minor fixes and updates
postdeployment
</commit_message>
<xml_diff>
--- a/templates/schedule_template.xlsx
+++ b/templates/schedule_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\xampp\htdocs\reserva-v2\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFF55A20-9958-4F49-89E7-AC3DBF79E0C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8151D780-C487-4865-9AF9-3B3DEA723860}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Subject Code</t>
   </si>
@@ -28,9 +28,6 @@
     <t>Subject</t>
   </si>
   <si>
-    <t>Days (e.g., Monday, Wednesday)</t>
-  </si>
-  <si>
     <t>Start Time (HH:MM AM/PM)</t>
   </si>
   <si>
@@ -40,28 +37,13 @@
     <t>Instructor</t>
   </si>
   <si>
-    <t>MATH101</t>
-  </si>
-  <si>
-    <t>ENG202</t>
-  </si>
-  <si>
-    <t>SCI303</t>
-  </si>
-  <si>
-    <t>Calculus I</t>
-  </si>
-  <si>
-    <t>English Literature</t>
-  </si>
-  <si>
-    <t>Physics</t>
-  </si>
-  <si>
     <t>Section</t>
   </si>
   <si>
-    <t xml:space="preserve"> Room Type</t>
+    <t>Day (e.g., Monday)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Room Type(Lecture, Laboratory)</t>
   </si>
 </sst>
 </file>
@@ -457,10 +439,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -483,49 +465,30 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="G1" s="1" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
         <v>7</v>
-      </c>
-      <c r="B3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" t="s">
-        <v>11</v>
       </c>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H3:H1048576 H2:H1048576" xr:uid="{16E61161-FC32-4ED6-9D49-C3DBA6651CF1}">
+      <formula1>"Lecture, Laboratory"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
minor fix and update
-room type has more types now
-drop downs minor update disabled first options
-added loader when reserving facility
-show sections that has uploaded schedules in current sem
-fixed room loading upload where time converted into decimal
-remove save button in account settings
-updated the schedule template
</commit_message>
<xml_diff>
--- a/templates/schedule_template.xlsx
+++ b/templates/schedule_template.xlsx
@@ -1,21 +1,38 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\xampp\htdocs\reserva-v2\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8151D780-C487-4865-9AF9-3B3DEA723860}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BB6D023-04E6-4ABD-98B1-5ABDF94FA5F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="TimeSlots" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <definedNames>
+    <definedName name="TimeSlots">TimeSlots!$A$1:$A$31</definedName>
+  </definedNames>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -43,13 +60,17 @@
     <t>Day (e.g., Monday)</t>
   </si>
   <si>
-    <t xml:space="preserve"> Room Type(Lecture, Laboratory)</t>
+    <t xml:space="preserve"> Room Type(Lecture,Computer Laboratory)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ am/pm"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -67,12 +88,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF66"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="4">
@@ -126,21 +153,30 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFFFF66"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -450,46 +486,256 @@
     <col min="1" max="1" width="15.28515625" customWidth="1"/>
     <col min="2" max="2" width="27.5703125" customWidth="1"/>
     <col min="3" max="3" width="26" customWidth="1"/>
-    <col min="4" max="4" width="18.140625" customWidth="1"/>
-    <col min="5" max="5" width="26.28515625" customWidth="1"/>
-    <col min="6" max="6" width="26.85546875" customWidth="1"/>
-    <col min="7" max="7" width="25" customWidth="1"/>
-    <col min="8" max="8" width="28.140625" customWidth="1"/>
+    <col min="4" max="4" width="28.42578125" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="18" style="5" customWidth="1"/>
+    <col min="7" max="7" width="19.42578125" customWidth="1"/>
+    <col min="8" max="8" width="37.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:8" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="4" t="s">
         <v>7</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H3:H1048576 H2:H1048576" xr:uid="{16E61161-FC32-4ED6-9D49-C3DBA6651CF1}">
-      <formula1>"Lecture, Laboratory"</formula1>
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E1048576 F2:F1048576" xr:uid="{A0BED604-4094-40B7-A7C9-1036CEFBC0F5}">
+      <formula1>TimeSlots</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2 G2:G1048576" xr:uid="{A0252E77-8014-451A-9177-B30098345DBA}">
+      <formula1>"Monday, Tuesday, Wednesday, Thursday, Friday, Saturday"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H1048576" xr:uid="{368A78AD-745C-4F47-980A-08A019288E2C}">
+      <formula1>"Lecture, Biology Laboratory, Chemistry Laboratory, Computer Laboratory, Electrical Engineering Laboratory, Electronics Engineering Laboratory, Fluid Mechanics Laboratory, Materials Testing Laboratory, Mechanical Engineering Laboratory, Physics Laboratory"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC4C535F-CAB3-462C-A101-EED2A3143DC6}">
+  <dimension ref="A1:A31"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1">
+        <v>0.29166666666666669</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <f>A1 + TIME(0,30,0)</f>
+        <v>0.3125</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <f t="shared" ref="A3:A31" si="0">A2 + TIME(0,30,0)</f>
+        <v>0.33333333333333331</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <f t="shared" si="0"/>
+        <v>0.35416666666666663</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <f t="shared" si="0"/>
+        <v>0.37499999999999994</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <f t="shared" si="0"/>
+        <v>0.39583333333333326</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <f t="shared" si="0"/>
+        <v>0.41666666666666657</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <f t="shared" si="0"/>
+        <v>0.43749999999999989</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <f t="shared" si="0"/>
+        <v>0.4583333333333332</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <f t="shared" si="0"/>
+        <v>0.47916666666666652</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <f t="shared" si="0"/>
+        <v>0.49999999999999983</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <f t="shared" si="0"/>
+        <v>0.52083333333333315</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <f t="shared" si="0"/>
+        <v>0.54166666666666652</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <f t="shared" si="0"/>
+        <v>0.56249999999999989</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <f t="shared" si="0"/>
+        <v>0.58333333333333326</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <f t="shared" si="0"/>
+        <v>0.60416666666666663</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <f t="shared" si="0"/>
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <f t="shared" si="0"/>
+        <v>0.64583333333333337</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <f t="shared" si="0"/>
+        <v>0.66666666666666674</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <f t="shared" si="0"/>
+        <v>0.68750000000000011</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <f>A20 + TIME(0,30,0)</f>
+        <v>0.70833333333333348</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <f t="shared" si="0"/>
+        <v>0.72916666666666685</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <f t="shared" si="0"/>
+        <v>0.75000000000000022</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <f t="shared" si="0"/>
+        <v>0.77083333333333359</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <f t="shared" si="0"/>
+        <v>0.79166666666666696</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <f t="shared" si="0"/>
+        <v>0.81250000000000033</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <f t="shared" si="0"/>
+        <v>0.8333333333333337</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <f t="shared" si="0"/>
+        <v>0.85416666666666707</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
+        <f t="shared" si="0"/>
+        <v>0.87500000000000044</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <f>A29 + TIME(0,30,0)</f>
+        <v>0.89583333333333381</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
+        <f t="shared" si="0"/>
+        <v>0.91666666666666718</v>
+      </c>
+    </row>
+  </sheetData>
+  <sheetProtection algorithmName="SHA-512" hashValue="6NnwxgUAb8h+n5HFDEQIQlFx8jmq2cMKbeYiB1g5nkJCAQSjha5A5RBTMTidobKphCH4hsTUbBvS7zCZzFEfpw==" saltValue="jjhOXTtkaws+vYQRi82jtQ==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>